<commit_message>
Solo falta exportar a sql
</commit_message>
<xml_diff>
--- a/input/Inventario de Datos Consolidado del ADN-Jun-2025-DSS.xlsx
+++ b/input/Inventario de Datos Consolidado del ADN-Jun-2025-DSS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francisco.fana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manuel.maldonado\Documents\Proyectos de Software\inventario_datos\excel\sistema_migracion_excel_inventario\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E758BAD3-B61C-4750-BCE7-D2D8BCE4E37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFC5D59-8448-4215-963D-FEF4111D0A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C08E161-1D32-48EC-AB54-AF37BA189D99}"/>
+    <workbookView xWindow="-28920" yWindow="4950" windowWidth="29040" windowHeight="15720" xr2:uid="{2C08E161-1D32-48EC-AB54-AF37BA189D99}"/>
   </bookViews>
   <sheets>
     <sheet name="Dir-Reportadas" sheetId="1" r:id="rId1"/>
@@ -53,17 +53,17 @@
   <commentList>
     <comment ref="B7" authorId="0" shapeId="0" xr:uid="{8E707B8C-FF3E-4212-966D-19039B3BD5B2}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar el nombre del archivo o base de datos que se refiere</t>
       </text>
     </comment>
     <comment ref="C7" authorId="1" shapeId="0" xr:uid="{0A7F57D8-E712-47AB-9938-324D38F7E805}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar lo que representa o describe
  la informacion a la que se regiere</t>
       </text>
@@ -84,9 +84,9 @@
     </comment>
     <comment ref="E7" authorId="3" shapeId="0" xr:uid="{2E151DDD-3814-4676-BD88-63D74BF3CA0B}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar quien es el responsable final o lider del Dato a que se refiere</t>
       </text>
     </comment>
@@ -239,17 +239,17 @@
     </comment>
     <comment ref="B111" authorId="4" shapeId="0" xr:uid="{87EC0FE1-6E30-4D1C-96B7-168616C13675}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar el nombre del archivo o base de datos que se refiere</t>
       </text>
     </comment>
     <comment ref="C111" authorId="5" shapeId="0" xr:uid="{D8FC64C4-0CD0-40BF-916D-B6304B94E6FC}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar lo que representa o describe
  la informacion a la que se regiere</t>
       </text>
@@ -270,9 +270,9 @@
     </comment>
     <comment ref="E111" authorId="6" shapeId="0" xr:uid="{D9AA7FAB-CD44-43AE-A1B7-33F8BC9B9808}">
       <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     Indicar quien es el responsable final o lider del Dato a que se refiere</t>
       </text>
     </comment>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="409">
   <si>
     <t>Ayuntamiento del Distrito Nacional</t>
   </si>
@@ -1558,9 +1558,6 @@
     <t>Area Administrativa de la Dirección</t>
   </si>
   <si>
-    <t>laudy.gonzález@adn.gob.do</t>
-  </si>
-  <si>
     <t>Laudys González (Auxiliar Administrativo)</t>
   </si>
   <si>
@@ -1576,9 +1573,6 @@
     <t>Area de Vacunación del Palacio Municipal</t>
   </si>
   <si>
-    <t>Ext. 1053 (Ramón Arias)</t>
-  </si>
-  <si>
     <t>Dr. Ramón Arias. (Encargado del Area de Vacunación)</t>
   </si>
   <si>
@@ -1597,9 +1591,6 @@
     <t>Departamento de Salud</t>
   </si>
   <si>
-    <t>Pablo Jhonson (829) 741-2617</t>
-  </si>
-  <si>
     <t>Dr. Pablo Jhonson (Encargado de Area de Salud)</t>
   </si>
   <si>
@@ -1615,9 +1606,6 @@
     <t>Areas de Lactancia</t>
   </si>
   <si>
-    <t>Yanely del Orbe Ext.1055</t>
-  </si>
-  <si>
     <t>Registro de visitas fisico</t>
   </si>
   <si>
@@ -1625,9 +1613,6 @@
   </si>
   <si>
     <t>Registro de las cantidades distribuidas en cada sector, para tener un record de las entregas.</t>
-  </si>
-  <si>
-    <t>Osvaldo.gonzalez@adn.gob.do</t>
   </si>
   <si>
     <t>Osvaldo Gonzalez (Soport Administrativo)</t>
@@ -1981,6 +1966,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2005,13 +1992,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -2074,9 +2059,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2114,7 +2099,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2220,7 +2205,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2362,7 +2347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2397,30 +2382,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BCA57-AE0F-4B76-912B-1109BD5D0C83}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A113" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A96" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112:E121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" customWidth="1"/>
+    <col min="3" max="3" width="96.453125" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" style="17" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="17" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="17"/>
-    <col min="15" max="15" width="13.85546875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="17" customWidth="1"/>
+    <col min="12" max="12" width="38.7265625" customWidth="1"/>
+    <col min="13" max="13" width="10.26953125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" style="17"/>
+    <col min="15" max="15" width="13.81640625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2437,83 +2422,83 @@
       <c r="N1" s="2"/>
       <c r="O1" s="20"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-    </row>
-    <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-    </row>
-    <row r="5" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-    </row>
-    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="14" t="s">
@@ -2521,23 +2506,23 @@
       </c>
       <c r="D6" s="15">
         <f ca="1">NOW()</f>
-        <v>45867.456441203707</v>
+        <v>45993.603557986113</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="36"/>
       <c r="N6" s="2"/>
       <c r="O6" s="20"/>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2584,7 +2569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -2629,7 +2614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -2674,7 +2659,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -2719,7 +2704,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -2764,7 +2749,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -2809,7 +2794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>6</v>
       </c>
@@ -2854,7 +2839,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>7</v>
       </c>
@@ -2901,7 +2886,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>8</v>
       </c>
@@ -2946,7 +2931,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>9</v>
       </c>
@@ -2981,7 +2966,7 @@
       <c r="N16" s="16"/>
       <c r="O16" s="22"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>10</v>
       </c>
@@ -3024,7 +3009,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>11</v>
       </c>
@@ -3069,7 +3054,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>12</v>
       </c>
@@ -3112,7 +3097,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>13</v>
       </c>
@@ -3157,7 +3142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>14</v>
       </c>
@@ -3202,7 +3187,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>15</v>
       </c>
@@ -3247,7 +3232,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>16</v>
       </c>
@@ -3290,7 +3275,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>17</v>
       </c>
@@ -3335,7 +3320,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>18</v>
       </c>
@@ -3380,7 +3365,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>19</v>
       </c>
@@ -3423,7 +3408,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>20</v>
       </c>
@@ -3466,7 +3451,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>21</v>
       </c>
@@ -3511,7 +3496,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>22</v>
       </c>
@@ -3556,7 +3541,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>23</v>
       </c>
@@ -3603,7 +3588,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>24</v>
       </c>
@@ -3646,7 +3631,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>25</v>
       </c>
@@ -3689,7 +3674,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>26</v>
       </c>
@@ -3734,7 +3719,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>27</v>
       </c>
@@ -3777,7 +3762,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>28</v>
       </c>
@@ -3820,7 +3805,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>29</v>
       </c>
@@ -3863,7 +3848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>30</v>
       </c>
@@ -3908,7 +3893,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>31</v>
       </c>
@@ -3951,7 +3936,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>32</v>
       </c>
@@ -3998,7 +3983,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>33</v>
       </c>
@@ -4045,7 +4030,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>34</v>
       </c>
@@ -4092,7 +4077,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>35</v>
       </c>
@@ -4139,7 +4124,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>36</v>
       </c>
@@ -4186,7 +4171,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>37</v>
       </c>
@@ -4233,7 +4218,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>38</v>
       </c>
@@ -4280,7 +4265,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>39</v>
       </c>
@@ -4327,7 +4312,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>40</v>
       </c>
@@ -4374,7 +4359,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>41</v>
       </c>
@@ -4409,7 +4394,7 @@
       <c r="N48" s="16"/>
       <c r="O48" s="22"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>42</v>
       </c>
@@ -4448,7 +4433,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43</v>
       </c>
@@ -4487,7 +4472,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>44</v>
       </c>
@@ -4526,7 +4511,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>45</v>
       </c>
@@ -4567,7 +4552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>46</v>
       </c>
@@ -4610,7 +4595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>47</v>
       </c>
@@ -4651,7 +4636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>48</v>
       </c>
@@ -4694,7 +4679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>49</v>
       </c>
@@ -4739,7 +4724,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>50</v>
       </c>
@@ -4784,7 +4769,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>51</v>
       </c>
@@ -4827,7 +4812,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>52</v>
       </c>
@@ -4872,7 +4857,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>53</v>
       </c>
@@ -4915,7 +4900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>54</v>
       </c>
@@ -4960,7 +4945,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>55</v>
       </c>
@@ -5007,7 +4992,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>56</v>
       </c>
@@ -5054,7 +5039,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>57</v>
       </c>
@@ -5099,7 +5084,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>58</v>
       </c>
@@ -5144,7 +5129,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>59</v>
       </c>
@@ -5189,7 +5174,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>60</v>
       </c>
@@ -5234,7 +5219,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>61</v>
       </c>
@@ -5281,7 +5266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>62</v>
       </c>
@@ -5328,7 +5313,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>63</v>
       </c>
@@ -5373,7 +5358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>64</v>
       </c>
@@ -5420,7 +5405,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>65</v>
       </c>
@@ -5465,7 +5450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>66</v>
       </c>
@@ -5510,7 +5495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>67</v>
       </c>
@@ -5555,7 +5540,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>68</v>
       </c>
@@ -5602,7 +5587,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>69</v>
       </c>
@@ -5649,7 +5634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>70</v>
       </c>
@@ -5696,7 +5681,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>71</v>
       </c>
@@ -5743,7 +5728,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>72</v>
       </c>
@@ -5788,7 +5773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>73</v>
       </c>
@@ -5833,7 +5818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>74</v>
       </c>
@@ -5878,7 +5863,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>75</v>
       </c>
@@ -5923,7 +5908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>76</v>
       </c>
@@ -5968,7 +5953,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>77</v>
       </c>
@@ -6013,7 +5998,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>78</v>
       </c>
@@ -6058,7 +6043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>79</v>
       </c>
@@ -6103,7 +6088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>80</v>
       </c>
@@ -6148,7 +6133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>81</v>
       </c>
@@ -6193,7 +6178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>82</v>
       </c>
@@ -6238,7 +6223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>83</v>
       </c>
@@ -6283,7 +6268,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>84</v>
       </c>
@@ -6328,7 +6313,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>85</v>
       </c>
@@ -6373,7 +6358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>86</v>
       </c>
@@ -6418,7 +6403,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>87</v>
       </c>
@@ -6463,7 +6448,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>88</v>
       </c>
@@ -6508,7 +6493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>89</v>
       </c>
@@ -6553,7 +6538,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>90</v>
       </c>
@@ -6598,7 +6583,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>91</v>
       </c>
@@ -6643,7 +6628,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>92</v>
       </c>
@@ -6688,7 +6673,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>93</v>
       </c>
@@ -6733,7 +6718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>94</v>
       </c>
@@ -6778,7 +6763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>95</v>
       </c>
@@ -6823,7 +6808,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" s="5">
         <v>96</v>
       </c>
@@ -6868,7 +6853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>97</v>
       </c>
@@ -6915,7 +6900,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>98</v>
       </c>
@@ -6960,7 +6945,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>99</v>
       </c>
@@ -6999,7 +6984,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>100</v>
       </c>
@@ -7044,7 +7029,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>101</v>
       </c>
@@ -7089,7 +7074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>102</v>
       </c>
@@ -7134,7 +7119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>103</v>
       </c>
@@ -7179,8 +7164,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="111" spans="1:15" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="35">
+    <row r="111" spans="1:15" s="30" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A111" s="29">
         <v>104</v>
       </c>
       <c r="B111" s="4" t="s">
@@ -7226,12 +7211,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>104</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>362</v>
@@ -7240,7 +7225,7 @@
         <v>363</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="F112" s="5">
         <v>45838</v>
@@ -7267,7 +7252,7 @@
       <c r="N112" s="16"/>
       <c r="O112" s="22"/>
     </row>
-    <row r="113" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A113" s="5">
         <v>105</v>
       </c>
@@ -7281,7 +7266,7 @@
         <v>370</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>371</v>
+        <v>341</v>
       </c>
       <c r="F113" s="5">
         <v>45838</v>
@@ -7308,7 +7293,7 @@
       <c r="N113" s="16"/>
       <c r="O113" s="22"/>
     </row>
-    <row r="114" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="5">
         <v>106</v>
       </c>
@@ -7322,7 +7307,7 @@
         <v>375</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="F114" s="5">
         <v>45838</v>
@@ -7331,7 +7316,7 @@
         <v>365</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I114" s="5" t="s">
         <v>44</v>
@@ -7340,7 +7325,7 @@
         <v>27</v>
       </c>
       <c r="K114" s="19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L114" s="5" t="s">
         <v>367</v>
@@ -7349,21 +7334,21 @@
       <c r="N114" s="16"/>
       <c r="O114" s="22"/>
     </row>
-    <row r="115" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="5">
         <v>107</v>
       </c>
       <c r="B115" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="C115" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="D115" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="D115" s="16" t="s">
-        <v>381</v>
-      </c>
       <c r="E115" s="5" t="s">
-        <v>382</v>
+        <v>341</v>
       </c>
       <c r="F115" s="5">
         <v>45838</v>
@@ -7372,7 +7357,7 @@
         <v>365</v>
       </c>
       <c r="H115" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I115" s="5" t="s">
         <v>44</v>
@@ -7381,30 +7366,30 @@
         <v>27</v>
       </c>
       <c r="K115" s="16" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L115" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M115" s="16"/>
       <c r="N115" s="16"/>
       <c r="O115" s="22"/>
     </row>
-    <row r="116" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="5">
         <v>108</v>
       </c>
       <c r="B116" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="D116" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="C116" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D116" s="16" t="s">
-        <v>388</v>
-      </c>
       <c r="E116" s="5" t="s">
-        <v>389</v>
+        <v>341</v>
       </c>
       <c r="F116" s="5">
         <v>45838</v>
@@ -7413,7 +7398,7 @@
         <v>365</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I116" s="5" t="s">
         <v>44</v>
@@ -7422,7 +7407,7 @@
         <v>27</v>
       </c>
       <c r="K116" s="16" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="L116" s="5" t="s">
         <v>367</v>
@@ -7431,21 +7416,21 @@
       <c r="N116" s="16"/>
       <c r="O116" s="22"/>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" s="5">
         <v>109</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D117" s="16" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>395</v>
+        <v>341</v>
       </c>
       <c r="F117" s="5">
         <v>45838</v>
@@ -7461,7 +7446,7 @@
         <v>27</v>
       </c>
       <c r="K117" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="L117" s="5" t="s">
         <v>367</v>
@@ -7470,21 +7455,21 @@
       <c r="N117" s="16"/>
       <c r="O117" s="22"/>
     </row>
-    <row r="118" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A118" s="5">
         <v>110</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D118" s="16" t="s">
         <v>375</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>399</v>
+        <v>341</v>
       </c>
       <c r="F118" s="5">
         <v>45746</v>
@@ -7493,7 +7478,7 @@
         <v>365</v>
       </c>
       <c r="H118" s="5" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>44</v>
@@ -7502,7 +7487,7 @@
         <v>27</v>
       </c>
       <c r="K118" s="16" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="L118" s="5" t="s">
         <v>367</v>
@@ -7511,21 +7496,21 @@
       <c r="N118" s="16"/>
       <c r="O118" s="22"/>
     </row>
-    <row r="119" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>111</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="D119" s="16" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="F119" s="5">
         <v>45838</v>
@@ -7534,7 +7519,7 @@
         <v>365</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I119" s="5" t="s">
         <v>44</v>
@@ -7543,7 +7528,7 @@
         <v>27</v>
       </c>
       <c r="K119" s="16" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="L119" s="5" t="s">
         <v>367</v>
@@ -7552,21 +7537,21 @@
       <c r="N119" s="16"/>
       <c r="O119" s="22"/>
     </row>
-    <row r="120" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>112</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D120" s="16" t="s">
         <v>375</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="F120" s="5">
         <v>45746</v>
@@ -7575,7 +7560,7 @@
         <v>365</v>
       </c>
       <c r="H120" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>44</v>
@@ -7584,7 +7569,7 @@
         <v>27</v>
       </c>
       <c r="K120" s="16" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="L120" s="5" t="s">
         <v>367</v>
@@ -7593,28 +7578,28 @@
       <c r="N120" s="16"/>
       <c r="O120" s="22"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>113</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D121" s="16" t="s">
         <v>375</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>376</v>
+        <v>341</v>
       </c>
       <c r="F121" s="5"/>
       <c r="G121" s="5" t="s">
         <v>365</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I121" s="5" t="s">
         <v>44</v>
@@ -7623,10 +7608,10 @@
         <v>27</v>
       </c>
       <c r="K121" s="16" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="L121" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="M121" s="16"/>
       <c r="N121" s="16"/>
@@ -7675,13 +7660,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.54296875" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C2" s="26" t="s">
         <v>316</v>
       </c>
@@ -7689,7 +7674,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -7703,7 +7688,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>2</v>
       </c>
@@ -7717,7 +7702,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>3</v>
       </c>
@@ -7731,7 +7716,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>4</v>
       </c>
@@ -7745,7 +7730,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>5</v>
       </c>
@@ -7759,7 +7744,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>6</v>
       </c>
@@ -7773,7 +7758,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>7</v>
       </c>
@@ -7787,7 +7772,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>8</v>
       </c>
@@ -7801,7 +7786,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>9</v>
       </c>
@@ -7815,7 +7800,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>10</v>
       </c>
@@ -7829,7 +7814,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>11</v>
       </c>
@@ -7843,7 +7828,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>12</v>
       </c>
@@ -7857,7 +7842,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>13</v>
       </c>
@@ -7871,7 +7856,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>14</v>
       </c>
@@ -7885,7 +7870,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>15</v>
       </c>
@@ -7899,7 +7884,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D18">
         <v>16</v>
       </c>
@@ -7907,7 +7892,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D19">
         <v>17</v>
       </c>
@@ -7915,7 +7900,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D20">
         <v>18</v>
       </c>
@@ -7923,7 +7908,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C21" s="27">
         <f>15/(15+32)</f>
         <v>0.31914893617021278</v>
@@ -7935,7 +7920,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D22">
         <v>20</v>
       </c>
@@ -7943,7 +7928,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D23">
         <v>21</v>
       </c>
@@ -7951,7 +7936,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C24">
         <f>+B17+D34</f>
         <v>47</v>
@@ -7963,7 +7948,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D25">
         <v>23</v>
       </c>
@@ -7971,7 +7956,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D26">
         <v>24</v>
       </c>
@@ -7979,7 +7964,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D27">
         <v>25</v>
       </c>
@@ -7987,7 +7972,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D28">
         <v>26</v>
       </c>
@@ -7995,7 +7980,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D29">
         <v>27</v>
       </c>
@@ -8003,7 +7988,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D30">
         <v>28</v>
       </c>
@@ -8011,7 +7996,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D31">
         <v>29</v>
       </c>
@@ -8019,7 +8004,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D32">
         <v>30</v>
       </c>
@@ -8027,7 +8012,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="4:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D33">
         <v>31</v>
       </c>
@@ -8035,7 +8020,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="4:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D34">
         <v>32</v>
       </c>
@@ -8043,7 +8028,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
       <c r="E36" s="27">
         <f>32/(15+32)</f>
         <v>0.68085106382978722</v>
@@ -8069,181 +8054,181 @@
       <selection activeCell="C2" sqref="C2:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C2" s="25" t="s">
         <v>318</v>
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C3" s="25" t="s">
         <v>319</v>
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C4" s="25" t="s">
         <v>320</v>
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C5" s="25" t="s">
         <v>321</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C6" s="25" t="s">
         <v>322</v>
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C7" s="25" t="s">
         <v>323</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C8" s="25" t="s">
         <v>324</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C9" s="25" t="s">
         <v>325</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C10" s="25" t="s">
         <v>326</v>
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C11" s="25" t="s">
         <v>327</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C12" s="25" t="s">
         <v>328</v>
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C13" s="25" t="s">
         <v>329</v>
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C14" s="25" t="s">
         <v>330</v>
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C15" s="25" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="3:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C16" s="25" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C17" s="25" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C18" s="25" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C19" s="25" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C20" s="25" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="21" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C21" s="25" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="22" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C22" s="25" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C23" s="25" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C24" s="25" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="25" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C25" s="25" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="26" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C26" s="25" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C27" s="25" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C28" s="25" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C29" s="25" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="30" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C30" s="25" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="31" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C31" s="25" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C32" s="25" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C33" s="25" t="s">
         <v>349</v>
       </c>

</xml_diff>